<commit_message>
frekvens + høj amplitude
</commit_message>
<xml_diff>
--- a/Technical_Documentation/Risk management/Risk analysis.xlsx
+++ b/Technical_Documentation/Risk management/Risk analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fie_b\Documents\GitHub\ST6\Technical_Documentation\Risk management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81C1F3C-B925-405F-A752-482F1E8BDAAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCEB519-E5ED-41DC-906C-A212DC7F4360}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,11 +89,6 @@
     <t>VeTP#</t>
   </si>
   <si>
-    <t>UCon stimulates 
-at a frequency
-too high</t>
-  </si>
-  <si>
     <t>Nerve damage</t>
   </si>
   <si>
@@ -330,6 +325,11 @@
   <si>
     <t>UD-SRS-13
 UD-SRS-15</t>
+  </si>
+  <si>
+    <t>UCon stimulates 
+at a frequency
+too high in combination with a high amplitude</t>
   </si>
 </sst>
 </file>
@@ -833,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -868,7 +868,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>4</v>
@@ -889,7 +889,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N1" s="11"/>
       <c r="O1" s="12"/>
@@ -921,7 +921,7 @@
         <v>12</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="18" t="s">
@@ -942,19 +942,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="E3" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>16</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>17</v>
       </c>
       <c r="G3" s="23" t="s">
         <v>7</v>
@@ -970,10 +970,10 @@
         <v>8</v>
       </c>
       <c r="K3" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="21" t="s">
         <v>22</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>23</v>
       </c>
       <c r="M3" s="20">
         <v>3</v>
@@ -986,31 +986,31 @@
         <v>3</v>
       </c>
       <c r="P3" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R3" s="20"/>
     </row>
     <row r="4" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="D4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="E4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F4" s="20" t="s">
         <v>31</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="G4" s="22" t="s">
         <v>7</v>
@@ -1026,10 +1026,10 @@
         <v>10</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L4" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M4" s="20">
         <v>2</v>
@@ -1042,31 +1042,31 @@
         <v>6</v>
       </c>
       <c r="P4" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q4" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R4" s="20"/>
     </row>
     <row r="5" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="E5" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="F5" s="21" t="s">
         <v>40</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>41</v>
       </c>
       <c r="G5" s="22" t="s">
         <v>7</v>
@@ -1082,10 +1082,10 @@
         <v>5</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M5" s="20">
         <v>1</v>
@@ -1098,31 +1098,31 @@
         <v>3</v>
       </c>
       <c r="P5" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q5" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R5" s="20"/>
     </row>
     <row r="6" spans="1:18" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="21" t="s">
+      <c r="E6" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="21" t="s">
-        <v>45</v>
-      </c>
       <c r="F6" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>7</v>
@@ -1138,10 +1138,10 @@
         <v>12</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M6" s="20">
         <v>3</v>
@@ -1154,31 +1154,31 @@
         <v>6</v>
       </c>
       <c r="P6" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q6" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R6" s="20"/>
     </row>
     <row r="7" spans="1:18" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="21" t="s">
         <v>47</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>48</v>
       </c>
       <c r="G7" s="22" t="s">
         <v>7</v>
@@ -1194,46 +1194,46 @@
         <v>5</v>
       </c>
       <c r="K7" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="L7" s="21" t="s">
-        <v>57</v>
-      </c>
       <c r="M7" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N7" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O7" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P7" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q7" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R7" s="20"/>
     </row>
     <row r="8" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="C8" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="D8" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="E8" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="F8" s="21" t="s">
         <v>53</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>54</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>7</v>
@@ -1249,10 +1249,10 @@
         <v>12</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L8" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M8" s="20">
         <v>4</v>
@@ -1265,10 +1265,10 @@
         <v>4</v>
       </c>
       <c r="P8" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q8" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R8" s="20"/>
     </row>

</xml_diff>